<commit_message>
sampek cek detik ter-recover 20 node
</commit_message>
<xml_diff>
--- a/hasil ujicoba.xlsx
+++ b/hasil ujicoba.xlsx
@@ -809,23 +809,24 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I130"/>
+  <dimension ref="A1:J130"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A107" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H131" activeCellId="0" sqref="H131"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I34" activeCellId="0" sqref="I34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.4030612244898"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.7908163265306"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.5"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.3265306122449"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="23.3520408163265"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.1326530612245"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.5204081632653"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.0612244897959"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="22.9489795918367"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -928,7 +929,10 @@
         <f aca="false">(E5-B5)/B4*100</f>
         <v>97.427652733119</v>
       </c>
-      <c r="I5" s="0" t="s">
+      <c r="I5" s="0" t="n">
+        <v>0.099412</v>
+      </c>
+      <c r="J5" s="0" t="s">
         <v>12</v>
       </c>
     </row>
@@ -958,7 +962,10 @@
         <f aca="false">(E6-B6)/B4*100</f>
         <v>91.1575562700964</v>
       </c>
-      <c r="I6" s="0" t="s">
+      <c r="I6" s="0" t="n">
+        <v>0.095963</v>
+      </c>
+      <c r="J6" s="0" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1012,7 +1019,10 @@
         <f aca="false">(E8-B8)/B7*100</f>
         <v>49.49</v>
       </c>
-      <c r="I8" s="0" t="s">
+      <c r="I8" s="0" t="n">
+        <v>0.007739</v>
+      </c>
+      <c r="J8" s="0" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1042,7 +1052,10 @@
         <f aca="false">(E9-B9)/B7*100</f>
         <v>48.77</v>
       </c>
-      <c r="I9" s="0" t="s">
+      <c r="I9" s="0" t="n">
+        <v>0.008899</v>
+      </c>
+      <c r="J9" s="0" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1096,7 +1109,10 @@
         <f aca="false">(E11-B11)/B10*100</f>
         <v>96.5</v>
       </c>
-      <c r="I11" s="0" t="s">
+      <c r="I11" s="0" t="n">
+        <v>0.007025</v>
+      </c>
+      <c r="J11" s="0" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1126,7 +1142,10 @@
         <f aca="false">(E12-B12)/B10*100</f>
         <v>97.45</v>
       </c>
-      <c r="I12" s="0" t="s">
+      <c r="I12" s="0" t="n">
+        <v>0.007022</v>
+      </c>
+      <c r="J12" s="0" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1234,7 +1253,10 @@
         <f aca="false">(E18-B18)/B17*100</f>
         <v>72.9414217219095</v>
       </c>
-      <c r="I18" s="0" t="s">
+      <c r="I18" s="0" t="n">
+        <v>0.035871</v>
+      </c>
+      <c r="J18" s="0" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1264,7 +1286,10 @@
         <f aca="false">(E19-B19)/B17*100</f>
         <v>75.2970606629143</v>
       </c>
-      <c r="I19" s="0" t="s">
+      <c r="I19" s="0" t="n">
+        <v>0.052088</v>
+      </c>
+      <c r="J19" s="0" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1294,7 +1319,10 @@
         <f aca="false">(E20-B20)/B17*100</f>
         <v>72.9726912653742</v>
       </c>
-      <c r="I20" s="0" t="s">
+      <c r="I20" s="0" t="n">
+        <v>0.030953</v>
+      </c>
+      <c r="J20" s="0" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1324,7 +1352,10 @@
         <f aca="false">(E21-B21)/B17*100</f>
         <v>67.5526370648322</v>
       </c>
-      <c r="I21" s="0" t="s">
+      <c r="I21" s="0" t="n">
+        <v>0.037118</v>
+      </c>
+      <c r="J21" s="0" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1354,7 +1385,10 @@
         <f aca="false">(E22-B22)/B17*100</f>
         <v>69.251615593079</v>
       </c>
-      <c r="I22" s="0" t="s">
+      <c r="I22" s="0" t="n">
+        <v>0.036832</v>
+      </c>
+      <c r="J22" s="0" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1408,7 +1442,10 @@
         <f aca="false">(E24-B24)/B23*100</f>
         <v>78.2468209297478</v>
       </c>
-      <c r="I24" s="0" t="s">
+      <c r="I24" s="0" t="n">
+        <v>0.058625</v>
+      </c>
+      <c r="J24" s="0" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1438,7 +1475,10 @@
         <f aca="false">(E25-B25)/B23*100</f>
         <v>23.6501980404419</v>
       </c>
-      <c r="I25" s="0" t="s">
+      <c r="I25" s="0" t="n">
+        <v>0.040516</v>
+      </c>
+      <c r="J25" s="0" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1468,7 +1508,10 @@
         <f aca="false">(E26-B26)/B23*100</f>
         <v>71.96164269335</v>
       </c>
-      <c r="I26" s="0" t="s">
+      <c r="I26" s="0" t="n">
+        <v>0.036499</v>
+      </c>
+      <c r="J26" s="0" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1498,7 +1541,10 @@
         <f aca="false">(E27-B27)/B23*100</f>
         <v>69.5538878465708</v>
       </c>
-      <c r="I27" s="0" t="s">
+      <c r="I27" s="0" t="n">
+        <v>0.032611</v>
+      </c>
+      <c r="J27" s="0" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1528,7 +1574,10 @@
         <f aca="false">(E28-B28)/B23*100</f>
         <v>77.2461955388785</v>
       </c>
-      <c r="I28" s="0" t="s">
+      <c r="I28" s="0" t="n">
+        <v>0.041835</v>
+      </c>
+      <c r="J28" s="0" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1582,7 +1631,10 @@
         <f aca="false">(E30-B30)/B29*100</f>
         <v>60.1521784448614</v>
       </c>
-      <c r="I30" s="0" t="s">
+      <c r="I30" s="0" t="n">
+        <v>0.043467</v>
+      </c>
+      <c r="J30" s="0" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1612,7 +1664,10 @@
         <f aca="false">(E31-B31)/B29*100</f>
         <v>58.4948926412341</v>
       </c>
-      <c r="I31" s="0" t="s">
+      <c r="I31" s="0" t="n">
+        <v>0.044429</v>
+      </c>
+      <c r="J31" s="0" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1642,7 +1697,10 @@
         <f aca="false">(E32-B32)/B29*100</f>
         <v>68.7408797164895</v>
       </c>
-      <c r="I32" s="0" t="s">
+      <c r="I32" s="0" t="n">
+        <v>0.031393</v>
+      </c>
+      <c r="J32" s="0" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1672,7 +1730,10 @@
         <f aca="false">(E33-B33)/B29*100</f>
         <v>54.3985824473629</v>
       </c>
-      <c r="I33" s="0" t="s">
+      <c r="I33" s="0" t="n">
+        <v>0.034425</v>
+      </c>
+      <c r="J33" s="0" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1702,7 +1763,10 @@
         <f aca="false">(E34-B34)/B29*100</f>
         <v>73.7023139462164</v>
       </c>
-      <c r="I34" s="0" t="s">
+      <c r="I34" s="0" t="n">
+        <v>0.03065</v>
+      </c>
+      <c r="J34" s="0" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1806,7 +1870,7 @@
         <f aca="false">(E40-B40)/B39*100</f>
         <v>49.1423125794155</v>
       </c>
-      <c r="I40" s="0" t="s">
+      <c r="J40" s="0" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1836,7 +1900,7 @@
         <f aca="false">(E41-B41)/B39*100</f>
         <v>35.4828462515883</v>
       </c>
-      <c r="I41" s="0" t="s">
+      <c r="J41" s="0" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1866,7 +1930,7 @@
         <f aca="false">(E42-B42)/B39*100</f>
         <v>42.8737822956374</v>
       </c>
-      <c r="I42" s="0" t="s">
+      <c r="J42" s="0" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1896,7 +1960,7 @@
         <f aca="false">(E43-B43)/B39*100</f>
         <v>50.868276154172</v>
       </c>
-      <c r="I43" s="0" t="s">
+      <c r="J43" s="0" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1926,7 +1990,7 @@
         <f aca="false">(E44-B44)/B39*100</f>
         <v>61.9229140194833</v>
       </c>
-      <c r="I44" s="0" t="s">
+      <c r="J44" s="0" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1980,7 +2044,7 @@
         <f aca="false">(E46-B46)/B45*100</f>
         <v>38.6488775942397</v>
       </c>
-      <c r="I46" s="0" t="s">
+      <c r="J46" s="0" t="s">
         <v>39</v>
       </c>
     </row>
@@ -2010,7 +2074,7 @@
         <f aca="false">(E47-B47)/B45*100</f>
         <v>35.0698856416773</v>
       </c>
-      <c r="I47" s="0" t="s">
+      <c r="J47" s="0" t="s">
         <v>40</v>
       </c>
     </row>
@@ -2040,7 +2104,7 @@
         <f aca="false">(E48-B48)/B45*100</f>
         <v>29.277848369335</v>
       </c>
-      <c r="I48" s="0" t="s">
+      <c r="J48" s="0" t="s">
         <v>41</v>
       </c>
     </row>
@@ -2070,7 +2134,7 @@
         <f aca="false">(E49-B49)/B45*100</f>
         <v>39.707750952986</v>
       </c>
-      <c r="I49" s="0" t="s">
+      <c r="J49" s="0" t="s">
         <v>42</v>
       </c>
     </row>
@@ -2100,7 +2164,7 @@
         <f aca="false">(E50-B50)/B45*100</f>
         <v>47.8822532825074</v>
       </c>
-      <c r="I50" s="0" t="s">
+      <c r="J50" s="0" t="s">
         <v>43</v>
       </c>
     </row>
@@ -2154,7 +2218,7 @@
         <f aca="false">(E52-B52)/B51*100</f>
         <v>33.8310038119441</v>
       </c>
-      <c r="I52" s="0" t="s">
+      <c r="J52" s="0" t="s">
         <v>44</v>
       </c>
     </row>
@@ -2184,7 +2248,7 @@
         <f aca="false">(E53-B53)/B51*100</f>
         <v>27.3401101228293</v>
       </c>
-      <c r="I53" s="0" t="s">
+      <c r="J53" s="0" t="s">
         <v>39</v>
       </c>
     </row>
@@ -2214,7 +2278,7 @@
         <f aca="false">(E54-B54)/B51*100</f>
         <v>44.9491740787802</v>
       </c>
-      <c r="I54" s="0" t="s">
+      <c r="J54" s="0" t="s">
         <v>45</v>
       </c>
     </row>
@@ -2244,7 +2308,7 @@
         <f aca="false">(E55-B55)/B51*100</f>
         <v>33.3545108005083</v>
       </c>
-      <c r="I55" s="0" t="s">
+      <c r="J55" s="0" t="s">
         <v>46</v>
       </c>
     </row>
@@ -2274,7 +2338,7 @@
         <f aca="false">(E56-B56)/B51*100</f>
         <v>44.0279542566709</v>
       </c>
-      <c r="I56" s="0" t="s">
+      <c r="J56" s="0" t="s">
         <v>47</v>
       </c>
     </row>
@@ -2382,7 +2446,7 @@
         <f aca="false">(E62-B62)/B61*100</f>
         <v>46.4360902255639</v>
       </c>
-      <c r="I62" s="0" t="s">
+      <c r="J62" s="0" t="s">
         <v>16</v>
       </c>
     </row>
@@ -2412,7 +2476,7 @@
         <f aca="false">(E63-B63)/B61*100</f>
         <v>25.4285714285714</v>
       </c>
-      <c r="I63" s="0" t="s">
+      <c r="J63" s="0" t="s">
         <v>49</v>
       </c>
     </row>
@@ -2442,7 +2506,7 @@
         <f aca="false">(E64-B64)/B61*100</f>
         <v>47.6390977443609</v>
       </c>
-      <c r="I64" s="0" t="s">
+      <c r="J64" s="0" t="s">
         <v>50</v>
       </c>
     </row>
@@ -2472,7 +2536,7 @@
         <f aca="false">(E65-B65)/B61*100</f>
         <v>19.7593984962406</v>
       </c>
-      <c r="I65" s="0" t="s">
+      <c r="J65" s="0" t="s">
         <v>51</v>
       </c>
     </row>
@@ -2502,7 +2566,7 @@
         <f aca="false">(E66-B66)/B61*100</f>
         <v>27.578947368421</v>
       </c>
-      <c r="I66" s="0" t="s">
+      <c r="J66" s="0" t="s">
         <v>52</v>
       </c>
     </row>
@@ -2532,7 +2596,7 @@
         <f aca="false">(E67-B67)/B61*100</f>
         <v>26.812030075188</v>
       </c>
-      <c r="I67" s="0" t="s">
+      <c r="J67" s="0" t="s">
         <v>54</v>
       </c>
     </row>
@@ -2562,7 +2626,7 @@
         <f aca="false">(E68-B68)/B61*100</f>
         <v>26.6015037593985</v>
       </c>
-      <c r="I68" s="0" t="s">
+      <c r="J68" s="0" t="s">
         <v>56</v>
       </c>
     </row>
@@ -2592,7 +2656,7 @@
         <f aca="false">(E69-B69)/B61*100</f>
         <v>31.0375939849624</v>
       </c>
-      <c r="I69" s="0" t="s">
+      <c r="J69" s="0" t="s">
         <v>58</v>
       </c>
     </row>
@@ -2622,7 +2686,7 @@
         <f aca="false">(E70-B70)/B61*100</f>
         <v>26.6766917293233</v>
       </c>
-      <c r="I70" s="0" t="s">
+      <c r="J70" s="0" t="s">
         <v>60</v>
       </c>
     </row>
@@ -2652,7 +2716,7 @@
         <f aca="false">(E71-B71)/B61*100</f>
         <v>26.5263157894737</v>
       </c>
-      <c r="I71" s="0" t="s">
+      <c r="J71" s="0" t="s">
         <v>62</v>
       </c>
     </row>
@@ -2706,7 +2770,7 @@
         <f aca="false">(E73-B73)/B72*100</f>
         <v>51.2932330827068</v>
       </c>
-      <c r="I73" s="0" t="s">
+      <c r="J73" s="0" t="s">
         <v>63</v>
       </c>
     </row>
@@ -2736,7 +2800,7 @@
         <f aca="false">(E74-B74)/B72*100</f>
         <v>27.9097744360902</v>
       </c>
-      <c r="I74" s="0" t="s">
+      <c r="J74" s="0" t="s">
         <v>18</v>
       </c>
     </row>
@@ -2766,7 +2830,7 @@
         <f aca="false">(E75-B75)/B72*100</f>
         <v>63.203007518797</v>
       </c>
-      <c r="I75" s="0" t="s">
+      <c r="J75" s="0" t="s">
         <v>64</v>
       </c>
     </row>
@@ -2796,7 +2860,7 @@
         <f aca="false">(E76-B76)/B72*100</f>
         <v>53.984962406015</v>
       </c>
-      <c r="I76" s="0" t="s">
+      <c r="J76" s="0" t="s">
         <v>65</v>
       </c>
     </row>
@@ -2826,7 +2890,7 @@
         <f aca="false">(E77-B77)/B72*100</f>
         <v>75.4436090225564</v>
       </c>
-      <c r="I77" s="0" t="s">
+      <c r="J77" s="0" t="s">
         <v>64</v>
       </c>
     </row>
@@ -2856,7 +2920,7 @@
         <f aca="false">(E78-B78)/B72*100</f>
         <v>61.3233082706767</v>
       </c>
-      <c r="I78" s="0" t="s">
+      <c r="J78" s="0" t="s">
         <v>66</v>
       </c>
     </row>
@@ -2886,7 +2950,7 @@
         <f aca="false">(E79-B79)/B72*100</f>
         <v>55.8345864661654</v>
       </c>
-      <c r="I79" s="0" t="s">
+      <c r="J79" s="0" t="s">
         <v>67</v>
       </c>
     </row>
@@ -2916,7 +2980,7 @@
         <f aca="false">(E80-B80)/B72*100</f>
         <v>76.2857142857143</v>
       </c>
-      <c r="I80" s="0" t="s">
+      <c r="J80" s="0" t="s">
         <v>68</v>
       </c>
     </row>
@@ -2946,7 +3010,7 @@
         <f aca="false">(E81-B81)/B72*100</f>
         <v>46.1654135338346</v>
       </c>
-      <c r="I81" s="0" t="s">
+      <c r="J81" s="0" t="s">
         <v>69</v>
       </c>
     </row>
@@ -3027,7 +3091,7 @@
         <f aca="false">(E84-B84)/B83*100</f>
         <v>35.1961777906472</v>
       </c>
-      <c r="I84" s="0" t="s">
+      <c r="J84" s="0" t="s">
         <v>49</v>
       </c>
     </row>
@@ -3057,7 +3121,7 @@
         <f aca="false">(E85-B85)/B83*100</f>
         <v>36.4992037063848</v>
       </c>
-      <c r="I85" s="0" t="s">
+      <c r="J85" s="0" t="s">
         <v>40</v>
       </c>
     </row>
@@ -3087,7 +3151,7 @@
         <f aca="false">(E86-B86)/B83*100</f>
         <v>50.1954538873607</v>
       </c>
-      <c r="I86" s="0" t="s">
+      <c r="J86" s="0" t="s">
         <v>70</v>
       </c>
     </row>
@@ -3117,7 +3181,7 @@
         <f aca="false">(E87-B87)/B83*100</f>
         <v>63.7903576082235</v>
       </c>
-      <c r="I87" s="0" t="s">
+      <c r="J87" s="0" t="s">
         <v>71</v>
       </c>
     </row>
@@ -3147,7 +3211,7 @@
         <f aca="false">(E88-B88)/B83*100</f>
         <v>37.2954973215578</v>
       </c>
-      <c r="I88" s="0" t="s">
+      <c r="J88" s="0" t="s">
         <v>72</v>
       </c>
     </row>
@@ -3177,7 +3241,7 @@
         <f aca="false">(E89-B89)/B83*100</f>
         <v>50.1664977558998</v>
       </c>
-      <c r="I89" s="0" t="s">
+      <c r="J89" s="0" t="s">
         <v>73</v>
       </c>
     </row>
@@ -3207,7 +3271,7 @@
         <f aca="false">(E90-B90)/B83*100</f>
         <v>50.2099319530911</v>
       </c>
-      <c r="I90" s="0" t="s">
+      <c r="J90" s="0" t="s">
         <v>74</v>
       </c>
     </row>
@@ -3237,7 +3301,7 @@
         <f aca="false">(E91-B91)/B83*100</f>
         <v>54.4664832778341</v>
       </c>
-      <c r="I91" s="0" t="s">
+      <c r="J91" s="0" t="s">
         <v>75</v>
       </c>
     </row>
@@ -3267,7 +3331,7 @@
         <f aca="false">(E92-B92)/B83*100</f>
         <v>43.5789778485594</v>
       </c>
-      <c r="I92" s="0" t="s">
+      <c r="J92" s="0" t="s">
         <v>76</v>
       </c>
     </row>
@@ -3297,7 +3361,7 @@
         <f aca="false">(E93-B93)/B83*100</f>
         <v>46.6048935862169</v>
       </c>
-      <c r="I93" s="0" t="s">
+      <c r="J93" s="0" t="s">
         <v>77</v>
       </c>
     </row>
@@ -3401,7 +3465,7 @@
         <f aca="false">(E99-B99)/B98*100</f>
         <v>46.5310380803339</v>
       </c>
-      <c r="I99" s="0" t="s">
+      <c r="J99" s="0" t="s">
         <v>40</v>
       </c>
     </row>
@@ -3431,7 +3495,7 @@
         <f aca="false">(E100-B100)/B98*100</f>
         <v>23.4872196139802</v>
       </c>
-      <c r="I100" s="0" t="s">
+      <c r="J100" s="0" t="s">
         <v>40</v>
       </c>
     </row>
@@ -3461,7 +3525,7 @@
         <f aca="false">(E101-B101)/B98*100</f>
         <v>37.4413145539906</v>
       </c>
-      <c r="I101" s="0" t="s">
+      <c r="J101" s="0" t="s">
         <v>79</v>
       </c>
     </row>
@@ -3491,7 +3555,7 @@
         <f aca="false">(E102-B102)/B98*100</f>
         <v>26.7083985393845</v>
       </c>
-      <c r="I102" s="0" t="s">
+      <c r="J102" s="0" t="s">
         <v>80</v>
       </c>
     </row>
@@ -3521,7 +3585,7 @@
         <f aca="false">(E103-B103)/B98*100</f>
         <v>36.906624934794</v>
       </c>
-      <c r="I103" s="0" t="s">
+      <c r="J103" s="0" t="s">
         <v>80</v>
       </c>
     </row>
@@ -3551,7 +3615,7 @@
         <f aca="false">(E104-B104)/B98*100</f>
         <v>36.5414710485133</v>
       </c>
-      <c r="I104" s="0" t="s">
+      <c r="J104" s="0" t="s">
         <v>81</v>
       </c>
     </row>
@@ -3581,7 +3645,7 @@
         <f aca="false">(E105-B105)/B98*100</f>
         <v>27.282211789254</v>
       </c>
-      <c r="I105" s="0" t="s">
+      <c r="J105" s="0" t="s">
         <v>82</v>
       </c>
     </row>
@@ -3611,7 +3675,7 @@
         <f aca="false">(E106-B106)/B98*100</f>
         <v>36.0198226395409</v>
       </c>
-      <c r="I106" s="0" t="s">
+      <c r="J106" s="0" t="s">
         <v>83</v>
       </c>
     </row>
@@ -3641,7 +3705,7 @@
         <f aca="false">(E107-B107)/B98*100</f>
         <v>26.9170579029734</v>
       </c>
-      <c r="I107" s="0" t="s">
+      <c r="J107" s="0" t="s">
         <v>84</v>
       </c>
     </row>
@@ -3671,7 +3735,7 @@
         <f aca="false">(E108-B108)/B98*100</f>
         <v>40.2712571726656</v>
       </c>
-      <c r="I108" s="0" t="s">
+      <c r="J108" s="0" t="s">
         <v>85</v>
       </c>
     </row>
@@ -3725,7 +3789,7 @@
         <f aca="false">(E110-B110)/B109*100</f>
         <v>36.4730878186969</v>
       </c>
-      <c r="I110" s="0" t="s">
+      <c r="J110" s="0" t="s">
         <v>15</v>
       </c>
     </row>
@@ -3755,7 +3819,7 @@
         <f aca="false">(E111-B111)/B109*100</f>
         <v>26.2747875354108</v>
       </c>
-      <c r="I111" s="0" t="s">
+      <c r="J111" s="0" t="s">
         <v>86</v>
       </c>
     </row>
@@ -3785,7 +3849,7 @@
         <f aca="false">(E112-B112)/B109*100</f>
         <v>32.9792256846081</v>
       </c>
-      <c r="I112" s="0" t="s">
+      <c r="J112" s="0" t="s">
         <v>87</v>
       </c>
     </row>
@@ -3815,7 +3879,7 @@
         <f aca="false">(E113-B113)/B109*100</f>
         <v>25.6610009442871</v>
       </c>
-      <c r="I113" s="0" t="s">
+      <c r="J113" s="0" t="s">
         <v>88</v>
       </c>
     </row>
@@ -3845,7 +3909,7 @@
         <f aca="false">(E114-B114)/B109*100</f>
         <v>18.6732766761095</v>
       </c>
-      <c r="I114" s="0" t="s">
+      <c r="J114" s="0" t="s">
         <v>28</v>
       </c>
     </row>
@@ -3875,7 +3939,7 @@
         <f aca="false">(E115-B115)/B109*100</f>
         <v>46.8366383380548</v>
       </c>
-      <c r="I115" s="0" t="s">
+      <c r="J115" s="0" t="s">
         <v>89</v>
       </c>
     </row>
@@ -3905,7 +3969,7 @@
         <f aca="false">(E116-B116)/B109*100</f>
         <v>19.6175637393768</v>
       </c>
-      <c r="I116" s="0" t="s">
+      <c r="J116" s="0" t="s">
         <v>90</v>
       </c>
     </row>
@@ -3935,7 +3999,7 @@
         <f aca="false">(E117-B117)/B109*100</f>
         <v>46.4117091595845</v>
       </c>
-      <c r="I117" s="0" t="s">
+      <c r="J117" s="0" t="s">
         <v>91</v>
       </c>
     </row>
@@ -3965,7 +4029,7 @@
         <f aca="false">(E118-B118)/B109*100</f>
         <v>23.300283286119</v>
       </c>
-      <c r="I118" s="0" t="s">
+      <c r="J118" s="0" t="s">
         <v>92</v>
       </c>
     </row>
@@ -3995,7 +4059,7 @@
         <f aca="false">(E119-B119)/B109*100</f>
         <v>27.5495750708215</v>
       </c>
-      <c r="I119" s="0" t="s">
+      <c r="J119" s="0" t="s">
         <v>93</v>
       </c>
     </row>
@@ -4049,7 +4113,7 @@
         <f aca="false">(E121-B121)/B120*100</f>
         <v>25.519357884797</v>
       </c>
-      <c r="I121" s="0" t="s">
+      <c r="J121" s="0" t="s">
         <v>18</v>
       </c>
     </row>
@@ -4079,7 +4143,7 @@
         <f aca="false">(E122-B122)/B120*100</f>
         <v>20.4674220963173</v>
       </c>
-      <c r="I122" s="0" t="s">
+      <c r="J122" s="0" t="s">
         <v>34</v>
       </c>
     </row>
@@ -4109,7 +4173,7 @@
         <f aca="false">(E123-B123)/B120*100</f>
         <v>21.4825306893296</v>
       </c>
-      <c r="I123" s="0" t="s">
+      <c r="J123" s="0" t="s">
         <v>94</v>
       </c>
     </row>
@@ -4139,7 +4203,7 @@
         <f aca="false">(E124-B124)/B120*100</f>
         <v>20.2785646836638</v>
       </c>
-      <c r="I124" s="0" t="s">
+      <c r="J124" s="0" t="s">
         <v>95</v>
       </c>
     </row>
@@ -4169,7 +4233,7 @@
         <f aca="false">(E125-B125)/B120*100</f>
         <v>16.6666666666667</v>
       </c>
-      <c r="I125" s="0" t="s">
+      <c r="J125" s="0" t="s">
         <v>96</v>
       </c>
     </row>
@@ -4199,7 +4263,7 @@
         <f aca="false">(E126-B126)/B120*100</f>
         <v>21.6949952785647</v>
       </c>
-      <c r="I126" s="0" t="s">
+      <c r="J126" s="0" t="s">
         <v>97</v>
       </c>
     </row>
@@ -4229,7 +4293,7 @@
         <f aca="false">(E127-B127)/B120*100</f>
         <v>15.9348441926346</v>
       </c>
-      <c r="I127" s="0" t="s">
+      <c r="J127" s="0" t="s">
         <v>98</v>
       </c>
     </row>
@@ -4259,7 +4323,7 @@
         <f aca="false">(E128-B128)/B120*100</f>
         <v>16.5486307837583</v>
       </c>
-      <c r="I128" s="0" t="s">
+      <c r="J128" s="0" t="s">
         <v>99</v>
       </c>
     </row>
@@ -4289,7 +4353,7 @@
         <f aca="false">(E129-B129)/B120*100</f>
         <v>15.9112370160529</v>
       </c>
-      <c r="I129" s="0" t="s">
+      <c r="J129" s="0" t="s">
         <v>100</v>
       </c>
     </row>
@@ -4319,7 +4383,7 @@
         <f aca="false">(E130-B130)/B120*100</f>
         <v>13.9518413597734</v>
       </c>
-      <c r="I130" s="0" t="s">
+      <c r="J130" s="0" t="s">
         <v>101</v>
       </c>
     </row>

</xml_diff>